<commit_message>
Added a new/missing hospital
</commit_message>
<xml_diff>
--- a/preprocess/data/raw/scotland-hospital-indicator-list.xlsx
+++ b/preprocess/data/raw/scotland-hospital-indicator-list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\040026704\Documents\Data science\Projects\nhs-capacity\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\040026704\Documents\Data science\Projects\nhs-capacity\preprocess\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A422106-3CDB-450B-A7C9-6FB5DB22FC51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE55FAC-71F3-4740-89D6-93768A8D3EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-4800" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Indicators" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="433">
   <si>
     <t xml:space="preserve">Emergency Department Activity (main sites) </t>
   </si>
@@ -1105,9 +1105,6 @@
     <t>S13002599</t>
   </si>
   <si>
-    <t>National</t>
-  </si>
-  <si>
     <t>D102H</t>
   </si>
   <si>
@@ -1313,6 +1310,21 @@
   </si>
   <si>
     <t>SteÃ²rnabhagh a Tuath</t>
+  </si>
+  <si>
+    <t>Golden Jubilee Foundation</t>
+  </si>
+  <si>
+    <t>Royal Hospital for Children and Young People</t>
+  </si>
+  <si>
+    <t>50 Little France Crescent, Edinburgh, EH16 4TJ</t>
+  </si>
+  <si>
+    <t>S319H</t>
+  </si>
+  <si>
+    <t>EH16 4TJ</t>
   </si>
 </sst>
 </file>
@@ -2014,13 +2026,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AF52F90-401F-420B-9BD6-341B13B973EC}">
-  <dimension ref="A1:V42"/>
+  <dimension ref="A1:V43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:V42"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -4271,67 +4305,19 @@
         <v>315</v>
       </c>
       <c r="B34" t="s">
-        <v>342</v>
+        <v>431</v>
       </c>
       <c r="C34" t="s">
-        <v>343</v>
+        <v>429</v>
       </c>
       <c r="D34" t="s">
-        <v>344</v>
+        <v>430</v>
       </c>
       <c r="E34">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="F34" t="s">
-        <v>345</v>
-      </c>
-      <c r="G34">
-        <v>-3.5230890000000001</v>
-      </c>
-      <c r="H34">
-        <v>55.891888000000002</v>
-      </c>
-      <c r="I34" t="s">
-        <v>67</v>
-      </c>
-      <c r="J34" t="s">
-        <v>68</v>
-      </c>
-      <c r="K34" t="s">
-        <v>346</v>
-      </c>
-      <c r="L34" t="s">
-        <v>347</v>
-      </c>
-      <c r="M34" t="s">
-        <v>348</v>
-      </c>
-      <c r="N34" t="s">
-        <v>349</v>
-      </c>
-      <c r="O34" t="s">
-        <v>350</v>
-      </c>
-      <c r="P34" t="s">
-        <v>351</v>
-      </c>
-      <c r="Q34" t="s">
-        <v>109</v>
-      </c>
-      <c r="R34">
-        <v>2</v>
-      </c>
-      <c r="S34">
-        <v>4123</v>
-      </c>
-      <c r="T34">
-        <v>6</v>
-      </c>
-      <c r="U34" t="s">
-        <v>110</v>
-      </c>
-      <c r="V34">
-        <v>9.6564616587445204</v>
+        <v>432</v>
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.25">
@@ -4339,25 +4325,25 @@
         <v>315</v>
       </c>
       <c r="B35" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="C35" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="D35" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="E35">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F35" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="G35">
-        <v>-3.1359379999999999</v>
+        <v>-3.5230890000000001</v>
       </c>
       <c r="H35">
-        <v>55.921759000000002</v>
+        <v>55.891888000000002</v>
       </c>
       <c r="I35" t="s">
         <v>67</v>
@@ -4366,66 +4352,66 @@
         <v>68</v>
       </c>
       <c r="K35" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="L35" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="M35" t="s">
-        <v>332</v>
+        <v>348</v>
       </c>
       <c r="N35" t="s">
-        <v>333</v>
+        <v>349</v>
       </c>
       <c r="O35" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="P35" t="s">
-        <v>74</v>
+        <v>351</v>
       </c>
       <c r="Q35" t="s">
-        <v>75</v>
+        <v>109</v>
       </c>
       <c r="R35">
+        <v>2</v>
+      </c>
+      <c r="S35">
+        <v>4123</v>
+      </c>
+      <c r="T35">
         <v>6</v>
       </c>
-      <c r="S35">
-        <v>1060</v>
-      </c>
-      <c r="T35">
-        <v>2</v>
-      </c>
       <c r="U35" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="V35">
-        <v>4.6281890286169203</v>
+        <v>9.6564616587445204</v>
       </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>359</v>
+        <v>315</v>
       </c>
       <c r="B36" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="C36" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="D36" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="E36">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="F36" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="G36">
-        <v>-4.4200030000000003</v>
+        <v>-3.1359379999999999</v>
       </c>
       <c r="H36">
-        <v>55.906460000000003</v>
+        <v>55.921759000000002</v>
       </c>
       <c r="I36" t="s">
         <v>67</v>
@@ -4434,66 +4420,66 @@
         <v>68</v>
       </c>
       <c r="K36" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="L36" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="M36" t="s">
-        <v>194</v>
+        <v>332</v>
       </c>
       <c r="N36" t="s">
-        <v>195</v>
+        <v>333</v>
       </c>
       <c r="O36" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="P36" t="s">
         <v>74</v>
       </c>
       <c r="Q36" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
       <c r="R36">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="S36">
-        <v>1749</v>
+        <v>1060</v>
       </c>
       <c r="T36">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U36" t="s">
-        <v>76</v>
+        <v>128</v>
       </c>
       <c r="V36">
-        <v>4.9489375284972201</v>
+        <v>4.6281890286169203</v>
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>367</v>
+        <v>428</v>
       </c>
       <c r="B37" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="C37" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="D37" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
       <c r="E37">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="F37" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="G37">
-        <v>-2.965624</v>
+        <v>-4.4200030000000003</v>
       </c>
       <c r="H37">
-        <v>58.976376999999999</v>
+        <v>55.906460000000003</v>
       </c>
       <c r="I37" t="s">
         <v>67</v>
@@ -4502,66 +4488,66 @@
         <v>68</v>
       </c>
       <c r="K37" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="L37" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="M37" t="s">
-        <v>374</v>
+        <v>194</v>
       </c>
       <c r="N37" t="s">
-        <v>375</v>
+        <v>195</v>
       </c>
       <c r="O37" t="s">
-        <v>376</v>
+        <v>365</v>
       </c>
       <c r="P37" t="s">
-        <v>377</v>
+        <v>74</v>
       </c>
       <c r="Q37" t="s">
         <v>109</v>
       </c>
       <c r="R37">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="S37">
-        <v>3411</v>
+        <v>1749</v>
       </c>
       <c r="T37">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="U37" t="s">
-        <v>155</v>
+        <v>76</v>
       </c>
       <c r="V37">
-        <v>6.5432835241805201</v>
+        <v>4.9489375284972201</v>
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>378</v>
+        <v>366</v>
       </c>
       <c r="B38" t="s">
-        <v>379</v>
+        <v>367</v>
       </c>
       <c r="C38" t="s">
-        <v>380</v>
+        <v>368</v>
       </c>
       <c r="D38" t="s">
-        <v>381</v>
+        <v>369</v>
       </c>
       <c r="E38">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="F38" t="s">
-        <v>382</v>
+        <v>370</v>
       </c>
       <c r="G38">
-        <v>-1.1556709999999999</v>
+        <v>-2.965624</v>
       </c>
       <c r="H38">
-        <v>60.151068000000002</v>
+        <v>58.976376999999999</v>
       </c>
       <c r="I38" t="s">
         <v>67</v>
@@ -4570,22 +4556,22 @@
         <v>68</v>
       </c>
       <c r="K38" t="s">
-        <v>383</v>
+        <v>371</v>
       </c>
       <c r="L38" t="s">
-        <v>384</v>
+        <v>372</v>
       </c>
       <c r="M38" t="s">
-        <v>385</v>
+        <v>373</v>
       </c>
       <c r="N38" t="s">
-        <v>386</v>
+        <v>374</v>
       </c>
       <c r="O38" t="s">
-        <v>387</v>
+        <v>375</v>
       </c>
       <c r="P38" t="s">
-        <v>388</v>
+        <v>376</v>
       </c>
       <c r="Q38" t="s">
         <v>109</v>
@@ -4594,42 +4580,42 @@
         <v>5</v>
       </c>
       <c r="S38">
-        <v>5395</v>
+        <v>3411</v>
       </c>
       <c r="T38">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="U38" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="V38">
-        <v>4.7450439808888598</v>
+        <v>6.5432835241805201</v>
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>389</v>
+        <v>377</v>
       </c>
       <c r="B39" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
       <c r="C39" t="s">
-        <v>391</v>
+        <v>379</v>
       </c>
       <c r="D39" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="E39">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F39" t="s">
-        <v>393</v>
+        <v>381</v>
       </c>
       <c r="G39">
-        <v>-2.991412</v>
+        <v>-1.1556709999999999</v>
       </c>
       <c r="H39">
-        <v>56.461688000000002</v>
+        <v>60.151068000000002</v>
       </c>
       <c r="I39" t="s">
         <v>67</v>
@@ -4638,66 +4624,66 @@
         <v>68</v>
       </c>
       <c r="K39" t="s">
-        <v>394</v>
+        <v>382</v>
       </c>
       <c r="L39" t="s">
-        <v>395</v>
+        <v>383</v>
       </c>
       <c r="M39" t="s">
-        <v>396</v>
+        <v>384</v>
       </c>
       <c r="N39" t="s">
-        <v>397</v>
+        <v>385</v>
       </c>
       <c r="O39" t="s">
-        <v>398</v>
+        <v>386</v>
       </c>
       <c r="P39" t="s">
-        <v>399</v>
+        <v>387</v>
       </c>
       <c r="Q39" t="s">
         <v>109</v>
       </c>
       <c r="R39">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="S39">
-        <v>2225</v>
+        <v>5395</v>
       </c>
       <c r="T39">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="U39" t="s">
-        <v>86</v>
+        <v>166</v>
       </c>
       <c r="V39">
-        <v>6.9522896610423004</v>
+        <v>4.7450439808888598</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>388</v>
+      </c>
+      <c r="B40" t="s">
         <v>389</v>
       </c>
-      <c r="B40" t="s">
-        <v>400</v>
-      </c>
       <c r="C40" t="s">
-        <v>401</v>
+        <v>390</v>
       </c>
       <c r="D40" t="s">
-        <v>402</v>
+        <v>391</v>
       </c>
       <c r="E40">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F40" t="s">
-        <v>403</v>
+        <v>392</v>
       </c>
       <c r="G40">
-        <v>-3.4529649999999998</v>
+        <v>-2.991412</v>
       </c>
       <c r="H40">
-        <v>56.396341</v>
+        <v>56.461688000000002</v>
       </c>
       <c r="I40" t="s">
         <v>67</v>
@@ -4706,66 +4692,66 @@
         <v>68</v>
       </c>
       <c r="K40" t="s">
-        <v>404</v>
+        <v>393</v>
       </c>
       <c r="L40" t="s">
-        <v>405</v>
+        <v>394</v>
       </c>
       <c r="M40" t="s">
-        <v>406</v>
+        <v>395</v>
       </c>
       <c r="N40" t="s">
-        <v>407</v>
+        <v>396</v>
       </c>
       <c r="O40" t="s">
-        <v>408</v>
+        <v>397</v>
       </c>
       <c r="P40" t="s">
-        <v>74</v>
+        <v>398</v>
       </c>
       <c r="Q40" t="s">
         <v>109</v>
       </c>
       <c r="R40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S40">
-        <v>6791</v>
+        <v>2225</v>
       </c>
       <c r="T40">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="U40" t="s">
-        <v>325</v>
+        <v>86</v>
       </c>
       <c r="V40">
-        <v>8.8210713402407208</v>
+        <v>6.9522896610423004</v>
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B41" t="s">
-        <v>409</v>
+        <v>399</v>
       </c>
       <c r="C41" t="s">
-        <v>410</v>
+        <v>400</v>
       </c>
       <c r="D41" t="s">
-        <v>411</v>
+        <v>401</v>
       </c>
       <c r="E41">
-        <v>71</v>
+        <v>28</v>
       </c>
       <c r="F41" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="G41">
-        <v>-2.6137199999999998</v>
+        <v>-3.4529649999999998</v>
       </c>
       <c r="H41">
-        <v>56.774940000000001</v>
+        <v>56.396341</v>
       </c>
       <c r="I41" t="s">
         <v>67</v>
@@ -4774,66 +4760,66 @@
         <v>68</v>
       </c>
       <c r="K41" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="L41" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
       <c r="M41" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
       <c r="N41" t="s">
-        <v>416</v>
+        <v>406</v>
       </c>
       <c r="O41" t="s">
-        <v>417</v>
+        <v>407</v>
       </c>
       <c r="P41" t="s">
         <v>74</v>
       </c>
       <c r="Q41" t="s">
-        <v>75</v>
+        <v>109</v>
       </c>
       <c r="R41">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="S41">
-        <v>4218</v>
+        <v>6791</v>
       </c>
       <c r="T41">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="U41" t="s">
-        <v>98</v>
+        <v>325</v>
       </c>
       <c r="V41">
-        <v>17.414157730748698</v>
+        <v>8.8210713402407208</v>
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>418</v>
+        <v>388</v>
       </c>
       <c r="B42" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="C42" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="D42" t="s">
-        <v>421</v>
+        <v>410</v>
       </c>
       <c r="E42">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="F42" t="s">
-        <v>422</v>
+        <v>411</v>
       </c>
       <c r="G42">
-        <v>-6.3844110000000001</v>
+        <v>-2.6137199999999998</v>
       </c>
       <c r="H42">
-        <v>58.221088000000002</v>
+        <v>56.774940000000001</v>
       </c>
       <c r="I42" t="s">
         <v>67</v>
@@ -4842,31 +4828,31 @@
         <v>68</v>
       </c>
       <c r="K42" t="s">
-        <v>423</v>
+        <v>412</v>
       </c>
       <c r="L42" t="s">
-        <v>424</v>
+        <v>413</v>
       </c>
       <c r="M42" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
       <c r="N42" t="s">
-        <v>426</v>
+        <v>415</v>
       </c>
       <c r="O42" t="s">
-        <v>427</v>
+        <v>416</v>
       </c>
       <c r="P42" t="s">
-        <v>428</v>
+        <v>74</v>
       </c>
       <c r="Q42" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
       <c r="R42">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="S42">
-        <v>4316</v>
+        <v>4218</v>
       </c>
       <c r="T42">
         <v>7</v>
@@ -4875,6 +4861,74 @@
         <v>98</v>
       </c>
       <c r="V42">
+        <v>17.414157730748698</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>417</v>
+      </c>
+      <c r="B43" t="s">
+        <v>418</v>
+      </c>
+      <c r="C43" t="s">
+        <v>419</v>
+      </c>
+      <c r="D43" t="s">
+        <v>420</v>
+      </c>
+      <c r="E43">
+        <v>49</v>
+      </c>
+      <c r="F43" t="s">
+        <v>421</v>
+      </c>
+      <c r="G43">
+        <v>-6.3844110000000001</v>
+      </c>
+      <c r="H43">
+        <v>58.221088000000002</v>
+      </c>
+      <c r="I43" t="s">
+        <v>67</v>
+      </c>
+      <c r="J43" t="s">
+        <v>68</v>
+      </c>
+      <c r="K43" t="s">
+        <v>422</v>
+      </c>
+      <c r="L43" t="s">
+        <v>423</v>
+      </c>
+      <c r="M43" t="s">
+        <v>424</v>
+      </c>
+      <c r="N43" t="s">
+        <v>425</v>
+      </c>
+      <c r="O43" t="s">
+        <v>426</v>
+      </c>
+      <c r="P43" t="s">
+        <v>427</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>109</v>
+      </c>
+      <c r="R43">
+        <v>5</v>
+      </c>
+      <c r="S43">
+        <v>4316</v>
+      </c>
+      <c r="T43">
+        <v>7</v>
+      </c>
+      <c r="U43" t="s">
+        <v>98</v>
+      </c>
+      <c r="V43">
         <v>8.1894353368250492</v>
       </c>
     </row>

</xml_diff>